<commit_message>
Unfortunately I had included 0% transmission power loss, so the QG18 just got a downgrade
</commit_message>
<xml_diff>
--- a/AC Worksheet v016 QG18DE.xlsx
+++ b/AC Worksheet v016 QG18DE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\LostInTranslationViewtModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B35F8C-29F4-48E7-8B25-6D07139BF547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE036C2F-D05F-4F10-8D07-E8EF67C13B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="629" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="411">
   <si>
     <t>Front Ride Height</t>
   </si>
@@ -1275,43 +1275,46 @@
     <t>Hankook  Ventus R-S4</t>
   </si>
   <si>
-    <t>0|0</t>
+    <t>1500|111</t>
   </si>
   <si>
-    <t>500|0</t>
+    <t>2000|122</t>
   </si>
   <si>
-    <t>1000|0</t>
+    <t>2500|130</t>
   </si>
   <si>
-    <t>1500|131</t>
+    <t>3000|136</t>
   </si>
   <si>
-    <t>2000|144</t>
+    <t>3500|134</t>
   </si>
   <si>
-    <t>2500|154</t>
+    <t>4000|136</t>
   </si>
   <si>
-    <t>3000|160</t>
+    <t>4500|140</t>
   </si>
   <si>
-    <t>4000|160</t>
+    <t>5000|138</t>
   </si>
   <si>
-    <t>4500|165</t>
+    <t>5500|136</t>
   </si>
   <si>
-    <t>5000|163</t>
+    <t>6000|119</t>
   </si>
   <si>
-    <t>5500|160</t>
+    <t>6500|110</t>
   </si>
   <si>
-    <t>6000|140</t>
+    <t>0|38</t>
   </si>
   <si>
-    <t>6500|130</t>
+    <t>500|38</t>
+  </si>
+  <si>
+    <t>1000|76</t>
   </si>
 </sst>
 </file>
@@ -3465,13 +3468,13 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3.1646482758620689</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.1646482758620689</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>12.658593103448275</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>27.63792827586207</c:v>
@@ -3748,46 +3751,46 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>38.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>38.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>76.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>131</c:v>
+                  <c:v>111.35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>144</c:v>
+                  <c:v>122.39999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>154</c:v>
+                  <c:v>130.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>160</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>158</c:v>
+                  <c:v>134.29999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>160</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>165</c:v>
+                  <c:v>140.25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>163</c:v>
+                  <c:v>138.54999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>160</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>140</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>130</c:v>
+                  <c:v>110.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -3890,6 +3893,12 @@
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>131</c:v>
@@ -13209,21 +13218,21 @@
       </c>
       <c r="H18" s="69">
         <f>H19</f>
-        <v>0</v>
+        <v>3.1646482758620689</v>
       </c>
       <c r="I18" s="77">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J18" s="72">
         <f>J19</f>
-        <v>0</v>
+        <v>38.25</v>
       </c>
       <c r="K18" s="22" t="str">
         <f t="shared" ref="K18:K54" si="0">CONCATENATE(D18,"|",INT(J18))</f>
-        <v>0|0</v>
+        <v>0|38</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
@@ -13265,24 +13274,26 @@
         <f t="shared" ref="F19:F54" si="1">E19*7.2330138512</f>
         <v>9</v>
       </c>
-      <c r="G19" s="62"/>
+      <c r="G19" s="62">
+        <v>45</v>
+      </c>
       <c r="H19" s="69">
         <f t="shared" ref="H19:H54" si="2">G19*0.101972*D19/725</f>
-        <v>0</v>
+        <v>3.1646482758620689</v>
       </c>
       <c r="I19" s="78">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J19" s="72">
         <f>G19*(1-I19)</f>
-        <v>0</v>
+        <v>38.25</v>
       </c>
       <c r="K19" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>500|0</v>
+        <v>500|38</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
@@ -13325,24 +13336,26 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="G20" s="62"/>
+      <c r="G20" s="62">
+        <v>90</v>
+      </c>
       <c r="H20" s="69">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>12.658593103448275</v>
       </c>
       <c r="I20" s="79">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J20" s="72">
         <f t="shared" ref="J20:J54" si="3">G20*(1-I20)</f>
-        <v>0</v>
+        <v>76.5</v>
       </c>
       <c r="K20" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>1000|0</v>
+        <v>1000|76</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>399</v>
+        <v>410</v>
       </c>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
@@ -13393,18 +13406,18 @@
         <v>27.63792827586207</v>
       </c>
       <c r="I21" s="79">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J21" s="72">
         <f t="shared" si="3"/>
-        <v>131</v>
+        <v>111.35</v>
       </c>
       <c r="K21" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>1500|131</v>
+        <v>1500|111</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
@@ -13455,18 +13468,18 @@
         <v>40.507497931034479</v>
       </c>
       <c r="I22" s="79">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J22" s="72">
         <f t="shared" si="3"/>
-        <v>144</v>
+        <v>122.39999999999999</v>
       </c>
       <c r="K22" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>2000|144</v>
+        <v>2000|122</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="M22" s="16"/>
       <c r="N22" s="16"/>
@@ -13517,18 +13530,18 @@
         <v>54.150648275862068</v>
       </c>
       <c r="I23" s="79">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J23" s="72">
         <f t="shared" si="3"/>
-        <v>154</v>
+        <v>130.9</v>
       </c>
       <c r="K23" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>2500|154</v>
+        <v>2500|130</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
@@ -13579,18 +13592,18 @@
         <v>67.512496551724141</v>
       </c>
       <c r="I24" s="79">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J24" s="72">
         <f t="shared" si="3"/>
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="K24" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>3000|160</v>
+        <v>3000|136</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
@@ -13641,18 +13654,18 @@
         <v>77.780022068965508</v>
       </c>
       <c r="I25" s="79">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J25" s="72">
         <f t="shared" si="3"/>
-        <v>158</v>
+        <v>134.29999999999998</v>
       </c>
       <c r="K25" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>3500|158</v>
+        <v>3500|134</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>360</v>
+        <v>401</v>
       </c>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
@@ -13703,18 +13716,18 @@
         <v>90.016662068965516</v>
       </c>
       <c r="I26" s="79">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J26" s="72">
         <f t="shared" si="3"/>
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="K26" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>4000|160</v>
+        <v>4000|136</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
@@ -13765,18 +13778,18 @@
         <v>104.43339310344827</v>
       </c>
       <c r="I27" s="79">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J27" s="72">
         <f t="shared" si="3"/>
-        <v>165</v>
+        <v>140.25</v>
       </c>
       <c r="K27" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>4500|165</v>
+        <v>4500|140</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
@@ -13827,18 +13840,18 @@
         <v>114.63059310344826</v>
       </c>
       <c r="I28" s="79">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J28" s="72">
         <f t="shared" si="3"/>
-        <v>163</v>
+        <v>138.54999999999998</v>
       </c>
       <c r="K28" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>5000|163</v>
+        <v>5000|138</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="M28" s="16"/>
       <c r="N28" s="16"/>
@@ -13889,18 +13902,18 @@
         <v>123.77291034482759</v>
       </c>
       <c r="I29" s="79">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J29" s="72">
         <f t="shared" si="3"/>
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="K29" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>5500|160</v>
+        <v>5500|136</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
@@ -13951,18 +13964,18 @@
         <v>118.14686896551724</v>
       </c>
       <c r="I30" s="79">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J30" s="72">
         <f t="shared" si="3"/>
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="K30" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>6000|140</v>
+        <v>6000|119</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="M30" s="16"/>
       <c r="N30" s="16"/>
@@ -14012,18 +14025,18 @@
         <v>118.85012413793103</v>
       </c>
       <c r="I31" s="79">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J31" s="72">
         <f t="shared" si="3"/>
-        <v>130</v>
+        <v>110.5</v>
       </c>
       <c r="K31" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>6500|130</v>
+        <v>6500|110</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
@@ -14066,7 +14079,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="62">
-        <f t="shared" ref="G20:G54" si="5">F32*1.35581794884</f>
+        <f t="shared" ref="G32:G54" si="5">F32*1.35581794884</f>
         <v>0</v>
       </c>
       <c r="H32" s="69">
@@ -14075,7 +14088,7 @@
       </c>
       <c r="I32" s="79">
         <f t="shared" ref="I32:I54" si="6">I31</f>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J32" s="72">
         <f t="shared" si="3"/>
@@ -14136,7 +14149,7 @@
       </c>
       <c r="I33" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J33" s="72">
         <f t="shared" si="3"/>
@@ -14197,7 +14210,7 @@
       </c>
       <c r="I34" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J34" s="72">
         <f t="shared" si="3"/>
@@ -14258,7 +14271,7 @@
       </c>
       <c r="I35" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J35" s="72">
         <f t="shared" si="3"/>
@@ -14319,7 +14332,7 @@
       </c>
       <c r="I36" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J36" s="72">
         <f t="shared" si="3"/>
@@ -14380,7 +14393,7 @@
       </c>
       <c r="I37" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J37" s="72">
         <f t="shared" si="3"/>
@@ -14441,7 +14454,7 @@
       </c>
       <c r="I38" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J38" s="72">
         <f t="shared" si="3"/>
@@ -14502,7 +14515,7 @@
       </c>
       <c r="I39" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J39" s="72">
         <f t="shared" si="3"/>
@@ -14563,7 +14576,7 @@
       </c>
       <c r="I40" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J40" s="72">
         <f t="shared" si="3"/>
@@ -14624,7 +14637,7 @@
       </c>
       <c r="I41" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J41" s="72">
         <f t="shared" si="3"/>
@@ -14685,7 +14698,7 @@
       </c>
       <c r="I42" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J42" s="72">
         <f t="shared" si="3"/>
@@ -14746,7 +14759,7 @@
       </c>
       <c r="I43" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J43" s="72">
         <f t="shared" si="3"/>
@@ -14807,7 +14820,7 @@
       </c>
       <c r="I44" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J44" s="72">
         <f t="shared" si="3"/>
@@ -14868,7 +14881,7 @@
       </c>
       <c r="I45" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J45" s="72">
         <f t="shared" si="3"/>
@@ -14929,7 +14942,7 @@
       </c>
       <c r="I46" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J46" s="72">
         <f t="shared" si="3"/>
@@ -14990,7 +15003,7 @@
       </c>
       <c r="I47" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J47" s="72">
         <f t="shared" si="3"/>
@@ -15051,7 +15064,7 @@
       </c>
       <c r="I48" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J48" s="72">
         <f t="shared" si="3"/>
@@ -15112,7 +15125,7 @@
       </c>
       <c r="I49" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J49" s="72">
         <f t="shared" si="3"/>
@@ -15173,7 +15186,7 @@
       </c>
       <c r="I50" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J50" s="72">
         <f t="shared" si="3"/>
@@ -15234,7 +15247,7 @@
       </c>
       <c r="I51" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J51" s="72">
         <f t="shared" si="3"/>
@@ -15295,7 +15308,7 @@
       </c>
       <c r="I52" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J52" s="72">
         <f t="shared" si="3"/>
@@ -15356,7 +15369,7 @@
       </c>
       <c r="I53" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J53" s="72">
         <f t="shared" si="3"/>
@@ -15417,7 +15430,7 @@
       </c>
       <c r="I54" s="79">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J54" s="72">
         <f t="shared" si="3"/>

</xml_diff>